<commit_message>
fixing adding to df errors
</commit_message>
<xml_diff>
--- a/Code/Photologic Rig Main Application Code/lineup.xlsx
+++ b/Code/Photologic Rig Main Application Code/lineup.xlsx
@@ -494,31 +494,31 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="G2" t="n">
-        <v>29150</v>
+        <v>33697</v>
       </c>
       <c r="H2" t="n">
-        <v>19734</v>
+        <v>17629</v>
       </c>
       <c r="I2" t="n">
-        <v>12234</v>
+        <v>18766</v>
       </c>
       <c r="J2" t="n">
-        <v>3802.408456802368</v>
+        <v>3956.982374191284</v>
       </c>
     </row>
     <row r="3">
@@ -530,31 +530,31 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>25205</v>
+        <v>26439</v>
       </c>
       <c r="H3" t="n">
-        <v>11348</v>
+        <v>10185</v>
       </c>
       <c r="I3" t="n">
-        <v>12908</v>
+        <v>13348</v>
       </c>
       <c r="J3" t="n">
-        <v>5970.19362449646</v>
+        <v>10185</v>
       </c>
     </row>
     <row r="4">
@@ -566,31 +566,31 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="G4" t="n">
-        <v>32776</v>
+        <v>26040</v>
       </c>
       <c r="H4" t="n">
-        <v>10362</v>
+        <v>17317</v>
       </c>
       <c r="I4" t="n">
-        <v>14190</v>
+        <v>16549</v>
       </c>
       <c r="J4" t="n">
-        <v>5565.382957458496</v>
+        <v>17317</v>
       </c>
     </row>
     <row r="5">
@@ -602,31 +602,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>water</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>21</v>
-      </c>
-      <c r="F5" t="n">
-        <v>23</v>
-      </c>
+          <t>lemon</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>31909</v>
+        <v>31111</v>
       </c>
       <c r="H5" t="n">
-        <v>11938</v>
+        <v>13371</v>
       </c>
       <c r="I5" t="n">
-        <v>16208</v>
+        <v>18862</v>
       </c>
       <c r="J5" t="n">
-        <v>7697.328090667725</v>
+        <v>5088.779926300049</v>
       </c>
     </row>
     <row r="6">
@@ -638,32 +634,26 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>bruh</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>44</v>
-      </c>
+          <t>fruit</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>26453</v>
+        <v>28552</v>
       </c>
       <c r="H6" t="n">
-        <v>11196</v>
+        <v>13103</v>
       </c>
       <c r="I6" t="n">
-        <v>11848</v>
-      </c>
-      <c r="J6" t="n">
-        <v>4381.550550460815</v>
-      </c>
+        <v>11704</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -674,32 +664,26 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>cake</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>28872</v>
+        <v>30151</v>
       </c>
       <c r="H7" t="n">
-        <v>15069</v>
+        <v>17856</v>
       </c>
       <c r="I7" t="n">
-        <v>16667</v>
-      </c>
-      <c r="J7" t="n">
-        <v>15069</v>
-      </c>
+        <v>17485</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -710,32 +694,26 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>fruit</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
+          <t>lime</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>34674</v>
+        <v>25252</v>
       </c>
       <c r="H8" t="n">
-        <v>17729</v>
+        <v>15000</v>
       </c>
       <c r="I8" t="n">
-        <v>12396</v>
-      </c>
-      <c r="J8" t="n">
-        <v>17729</v>
-      </c>
+        <v>14095</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -746,32 +724,26 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>water</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
+          <t>lemon</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>26718</v>
+        <v>27520</v>
       </c>
       <c r="H9" t="n">
-        <v>19857</v>
+        <v>11391</v>
       </c>
       <c r="I9" t="n">
-        <v>13376</v>
-      </c>
-      <c r="J9" t="n">
-        <v>19857</v>
-      </c>
+        <v>14069</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -782,32 +754,26 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>fruit</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
+          <t>lime</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>31567</v>
+        <v>34336</v>
       </c>
       <c r="H10" t="n">
-        <v>19323</v>
+        <v>15149</v>
       </c>
       <c r="I10" t="n">
-        <v>10161</v>
-      </c>
-      <c r="J10" t="n">
-        <v>19323</v>
-      </c>
+        <v>17743</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -818,32 +784,26 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>bruh</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
+          <t>fruit</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>31393</v>
+        <v>27395</v>
       </c>
       <c r="H11" t="n">
-        <v>16398</v>
+        <v>10109</v>
       </c>
       <c r="I11" t="n">
-        <v>16085</v>
-      </c>
-      <c r="J11" t="n">
-        <v>16398</v>
-      </c>
+        <v>16841</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -854,32 +814,26 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>water</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>26</v>
-      </c>
-      <c r="F12" t="n">
-        <v>22</v>
-      </c>
+          <t>lemon</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>27709</v>
+        <v>34694</v>
       </c>
       <c r="H12" t="n">
-        <v>18315</v>
+        <v>11952</v>
       </c>
       <c r="I12" t="n">
-        <v>17392</v>
-      </c>
-      <c r="J12" t="n">
-        <v>18315</v>
-      </c>
+        <v>13126</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -890,32 +844,26 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>cake</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
+          <t>water</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>33428</v>
+        <v>27288</v>
       </c>
       <c r="H13" t="n">
-        <v>13120</v>
+        <v>14032</v>
       </c>
       <c r="I13" t="n">
-        <v>18370</v>
-      </c>
-      <c r="J13" t="n">
-        <v>3025.736808776855</v>
-      </c>
+        <v>18054</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -926,28 +874,26 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>27231</v>
+        <v>29569</v>
       </c>
       <c r="H14" t="n">
-        <v>17846</v>
+        <v>10511</v>
       </c>
       <c r="I14" t="n">
-        <v>12107</v>
-      </c>
-      <c r="J14" t="n">
-        <v>4051.254510879517</v>
-      </c>
+        <v>19700</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -958,28 +904,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>29713</v>
+        <v>33058</v>
       </c>
       <c r="H15" t="n">
-        <v>14805</v>
+        <v>15816</v>
       </c>
       <c r="I15" t="n">
-        <v>15004</v>
-      </c>
-      <c r="J15" t="n">
-        <v>14805</v>
-      </c>
+        <v>15067</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -990,24 +934,24 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>28190</v>
+        <v>32696</v>
       </c>
       <c r="H16" t="n">
-        <v>11929</v>
+        <v>19085</v>
       </c>
       <c r="I16" t="n">
-        <v>17240</v>
+        <v>17859</v>
       </c>
       <c r="J16" t="inlineStr"/>
     </row>
@@ -1020,24 +964,24 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>29022</v>
+        <v>31069</v>
       </c>
       <c r="H17" t="n">
-        <v>13625</v>
+        <v>16674</v>
       </c>
       <c r="I17" t="n">
-        <v>11117</v>
+        <v>11883</v>
       </c>
       <c r="J17" t="inlineStr"/>
     </row>
@@ -1050,24 +994,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
-        <v>30706</v>
+        <v>28827</v>
       </c>
       <c r="H18" t="n">
-        <v>13138</v>
+        <v>11511</v>
       </c>
       <c r="I18" t="n">
-        <v>14561</v>
+        <v>14753</v>
       </c>
       <c r="J18" t="inlineStr"/>
     </row>
@@ -1080,24 +1024,24 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>27600</v>
+        <v>29197</v>
       </c>
       <c r="H19" t="n">
-        <v>13844</v>
+        <v>12703</v>
       </c>
       <c r="I19" t="n">
-        <v>19369</v>
+        <v>17897</v>
       </c>
       <c r="J19" t="inlineStr"/>
     </row>
@@ -1110,24 +1054,24 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>32245</v>
+        <v>32112</v>
       </c>
       <c r="H20" t="n">
-        <v>15352</v>
+        <v>12772</v>
       </c>
       <c r="I20" t="n">
-        <v>19545</v>
+        <v>18523</v>
       </c>
       <c r="J20" t="inlineStr"/>
     </row>
@@ -1140,24 +1084,24 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>31063</v>
+        <v>25696</v>
       </c>
       <c r="H21" t="n">
-        <v>13014</v>
+        <v>11562</v>
       </c>
       <c r="I21" t="n">
-        <v>17945</v>
+        <v>17474</v>
       </c>
       <c r="J21" t="inlineStr"/>
     </row>
@@ -1170,24 +1114,24 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>25190</v>
+        <v>28826</v>
       </c>
       <c r="H22" t="n">
-        <v>11137</v>
+        <v>11074</v>
       </c>
       <c r="I22" t="n">
-        <v>11245</v>
+        <v>12212</v>
       </c>
       <c r="J22" t="inlineStr"/>
     </row>
@@ -1200,24 +1144,24 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>32793</v>
+        <v>31822</v>
       </c>
       <c r="H23" t="n">
-        <v>19373</v>
+        <v>16964</v>
       </c>
       <c r="I23" t="n">
-        <v>13191</v>
+        <v>14118</v>
       </c>
       <c r="J23" t="inlineStr"/>
     </row>
@@ -1230,24 +1174,24 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>34464</v>
+        <v>33846</v>
       </c>
       <c r="H24" t="n">
-        <v>16176</v>
+        <v>10312</v>
       </c>
       <c r="I24" t="n">
-        <v>15863</v>
+        <v>14857</v>
       </c>
       <c r="J24" t="inlineStr"/>
     </row>
@@ -1260,24 +1204,24 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
-        <v>25664</v>
+        <v>34449</v>
       </c>
       <c r="H25" t="n">
-        <v>14720</v>
+        <v>10202</v>
       </c>
       <c r="I25" t="n">
-        <v>11785</v>
+        <v>13044</v>
       </c>
       <c r="J25" t="inlineStr"/>
     </row>
@@ -1290,24 +1234,24 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>30017</v>
+        <v>33574</v>
       </c>
       <c r="H26" t="n">
-        <v>16909</v>
+        <v>10518</v>
       </c>
       <c r="I26" t="n">
-        <v>16914</v>
+        <v>19953</v>
       </c>
       <c r="J26" t="inlineStr"/>
     </row>
@@ -1320,24 +1264,24 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>30860</v>
+        <v>33038</v>
       </c>
       <c r="H27" t="n">
-        <v>16315</v>
+        <v>17189</v>
       </c>
       <c r="I27" t="n">
-        <v>18466</v>
+        <v>17196</v>
       </c>
       <c r="J27" t="inlineStr"/>
     </row>
@@ -1350,24 +1294,24 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
-        <v>29325</v>
+        <v>34725</v>
       </c>
       <c r="H28" t="n">
-        <v>13917</v>
+        <v>17953</v>
       </c>
       <c r="I28" t="n">
-        <v>11535</v>
+        <v>13163</v>
       </c>
       <c r="J28" t="inlineStr"/>
     </row>
@@ -1380,24 +1324,24 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>31454</v>
+        <v>32036</v>
       </c>
       <c r="H29" t="n">
-        <v>12184</v>
+        <v>14007</v>
       </c>
       <c r="I29" t="n">
-        <v>18548</v>
+        <v>14484</v>
       </c>
       <c r="J29" t="inlineStr"/>
     </row>
@@ -1410,24 +1354,24 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>33143</v>
+        <v>31006</v>
       </c>
       <c r="H30" t="n">
-        <v>13850</v>
+        <v>17397</v>
       </c>
       <c r="I30" t="n">
-        <v>16143</v>
+        <v>16118</v>
       </c>
       <c r="J30" t="inlineStr"/>
     </row>
@@ -1440,24 +1384,24 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="n">
-        <v>28161</v>
+        <v>32843</v>
       </c>
       <c r="H31" t="n">
-        <v>18199</v>
+        <v>13324</v>
       </c>
       <c r="I31" t="n">
-        <v>19039</v>
+        <v>14977</v>
       </c>
       <c r="J31" t="inlineStr"/>
     </row>
@@ -1470,24 +1414,24 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>27819</v>
+        <v>30333</v>
       </c>
       <c r="H32" t="n">
-        <v>19096</v>
+        <v>17911</v>
       </c>
       <c r="I32" t="n">
-        <v>18193</v>
+        <v>18104</v>
       </c>
       <c r="J32" t="inlineStr"/>
     </row>
@@ -1500,24 +1444,24 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>29735</v>
+        <v>33195</v>
       </c>
       <c r="H33" t="n">
-        <v>13397</v>
+        <v>16726</v>
       </c>
       <c r="I33" t="n">
-        <v>11204</v>
+        <v>14487</v>
       </c>
       <c r="J33" t="inlineStr"/>
     </row>
@@ -1530,24 +1474,24 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>30902</v>
+        <v>29458</v>
       </c>
       <c r="H34" t="n">
-        <v>18529</v>
+        <v>10345</v>
       </c>
       <c r="I34" t="n">
-        <v>13935</v>
+        <v>18735</v>
       </c>
       <c r="J34" t="inlineStr"/>
     </row>
@@ -1560,24 +1504,24 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
-        <v>26474</v>
+        <v>26713</v>
       </c>
       <c r="H35" t="n">
-        <v>16189</v>
+        <v>10605</v>
       </c>
       <c r="I35" t="n">
-        <v>13431</v>
+        <v>19959</v>
       </c>
       <c r="J35" t="inlineStr"/>
     </row>
@@ -1590,24 +1534,24 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
-        <v>34323</v>
+        <v>32838</v>
       </c>
       <c r="H36" t="n">
-        <v>17703</v>
+        <v>16017</v>
       </c>
       <c r="I36" t="n">
-        <v>11396</v>
+        <v>15163</v>
       </c>
       <c r="J36" t="inlineStr"/>
     </row>
@@ -1620,24 +1564,24 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
-        <v>34879</v>
+        <v>26573</v>
       </c>
       <c r="H37" t="n">
-        <v>19900</v>
+        <v>19776</v>
       </c>
       <c r="I37" t="n">
-        <v>13214</v>
+        <v>11014</v>
       </c>
       <c r="J37" t="inlineStr"/>
     </row>
@@ -1650,24 +1594,24 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
-        <v>31634</v>
+        <v>31624</v>
       </c>
       <c r="H38" t="n">
-        <v>14993</v>
+        <v>10089</v>
       </c>
       <c r="I38" t="n">
-        <v>17019</v>
+        <v>10828</v>
       </c>
       <c r="J38" t="inlineStr"/>
     </row>
@@ -1680,24 +1624,24 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="n">
-        <v>26402</v>
+        <v>34559</v>
       </c>
       <c r="H39" t="n">
-        <v>17508</v>
+        <v>15709</v>
       </c>
       <c r="I39" t="n">
-        <v>14444</v>
+        <v>16794</v>
       </c>
       <c r="J39" t="inlineStr"/>
     </row>
@@ -1710,24 +1654,24 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
-        <v>27847</v>
+        <v>26996</v>
       </c>
       <c r="H40" t="n">
-        <v>19108</v>
+        <v>11334</v>
       </c>
       <c r="I40" t="n">
-        <v>12737</v>
+        <v>19813</v>
       </c>
       <c r="J40" t="inlineStr"/>
     </row>
@@ -1751,13 +1695,13 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="n">
-        <v>27338</v>
+        <v>31457</v>
       </c>
       <c r="H41" t="n">
-        <v>18738</v>
+        <v>10144</v>
       </c>
       <c r="I41" t="n">
-        <v>13846</v>
+        <v>12621</v>
       </c>
       <c r="J41" t="inlineStr"/>
     </row>
@@ -1770,24 +1714,24 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
-        <v>33860</v>
+        <v>29573</v>
       </c>
       <c r="H42" t="n">
-        <v>18749</v>
+        <v>19167</v>
       </c>
       <c r="I42" t="n">
-        <v>19802</v>
+        <v>15521</v>
       </c>
       <c r="J42" t="inlineStr"/>
     </row>
@@ -1800,24 +1744,24 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="n">
-        <v>30217</v>
+        <v>32700</v>
       </c>
       <c r="H43" t="n">
-        <v>17042</v>
+        <v>14089</v>
       </c>
       <c r="I43" t="n">
-        <v>12037</v>
+        <v>15268</v>
       </c>
       <c r="J43" t="inlineStr"/>
     </row>
@@ -1830,24 +1774,24 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>27613</v>
+        <v>31556</v>
       </c>
       <c r="H44" t="n">
-        <v>12045</v>
+        <v>10137</v>
       </c>
       <c r="I44" t="n">
-        <v>13196</v>
+        <v>16102</v>
       </c>
       <c r="J44" t="inlineStr"/>
     </row>
@@ -1860,24 +1804,24 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
-        <v>34752</v>
+        <v>31785</v>
       </c>
       <c r="H45" t="n">
-        <v>10218</v>
+        <v>13719</v>
       </c>
       <c r="I45" t="n">
-        <v>15080</v>
+        <v>13129</v>
       </c>
       <c r="J45" t="inlineStr"/>
     </row>
@@ -1890,24 +1834,24 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="n">
-        <v>32126</v>
+        <v>32592</v>
       </c>
       <c r="H46" t="n">
-        <v>15725</v>
+        <v>11058</v>
       </c>
       <c r="I46" t="n">
-        <v>15952</v>
+        <v>10647</v>
       </c>
       <c r="J46" t="inlineStr"/>
     </row>
@@ -1920,24 +1864,24 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
-        <v>29966</v>
+        <v>26893</v>
       </c>
       <c r="H47" t="n">
-        <v>19890</v>
+        <v>10058</v>
       </c>
       <c r="I47" t="n">
-        <v>16164</v>
+        <v>12524</v>
       </c>
       <c r="J47" t="inlineStr"/>
     </row>
@@ -1950,24 +1894,24 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="n">
-        <v>26199</v>
+        <v>30109</v>
       </c>
       <c r="H48" t="n">
-        <v>14757</v>
+        <v>19007</v>
       </c>
       <c r="I48" t="n">
-        <v>15356</v>
+        <v>18609</v>
       </c>
       <c r="J48" t="inlineStr"/>
     </row>
@@ -1980,24 +1924,24 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="n">
-        <v>29993</v>
+        <v>29049</v>
       </c>
       <c r="H49" t="n">
-        <v>17949</v>
+        <v>14833</v>
       </c>
       <c r="I49" t="n">
-        <v>16489</v>
+        <v>14582</v>
       </c>
       <c r="J49" t="inlineStr"/>
     </row>
@@ -2010,24 +1954,24 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="n">
-        <v>34337</v>
+        <v>30921</v>
       </c>
       <c r="H50" t="n">
-        <v>12789</v>
+        <v>14881</v>
       </c>
       <c r="I50" t="n">
-        <v>19825</v>
+        <v>19992</v>
       </c>
       <c r="J50" t="inlineStr"/>
     </row>
@@ -2040,24 +1984,24 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="n">
-        <v>27314</v>
+        <v>28724</v>
       </c>
       <c r="H51" t="n">
-        <v>13965</v>
+        <v>15318</v>
       </c>
       <c r="I51" t="n">
-        <v>14577</v>
+        <v>10809</v>
       </c>
       <c r="J51" t="inlineStr"/>
     </row>
@@ -2070,24 +2014,24 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>34369</v>
+        <v>28078</v>
       </c>
       <c r="H52" t="n">
-        <v>16647</v>
+        <v>11958</v>
       </c>
       <c r="I52" t="n">
-        <v>17878</v>
+        <v>10841</v>
       </c>
       <c r="J52" t="inlineStr"/>
     </row>
@@ -2100,24 +2044,24 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
-        <v>29169</v>
+        <v>28538</v>
       </c>
       <c r="H53" t="n">
-        <v>15298</v>
+        <v>17741</v>
       </c>
       <c r="I53" t="n">
-        <v>18985</v>
+        <v>19145</v>
       </c>
       <c r="J53" t="inlineStr"/>
     </row>
@@ -2130,24 +2074,24 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>29817</v>
+        <v>30976</v>
       </c>
       <c r="H54" t="n">
-        <v>19417</v>
+        <v>18780</v>
       </c>
       <c r="I54" t="n">
-        <v>11813</v>
+        <v>16356</v>
       </c>
       <c r="J54" t="inlineStr"/>
     </row>
@@ -2160,24 +2104,24 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
-        <v>31091</v>
+        <v>31507</v>
       </c>
       <c r="H55" t="n">
-        <v>17265</v>
+        <v>15010</v>
       </c>
       <c r="I55" t="n">
-        <v>15834</v>
+        <v>15336</v>
       </c>
       <c r="J55" t="inlineStr"/>
     </row>
@@ -2190,24 +2134,24 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
-        <v>31524</v>
+        <v>30439</v>
       </c>
       <c r="H56" t="n">
-        <v>17575</v>
+        <v>11459</v>
       </c>
       <c r="I56" t="n">
-        <v>13836</v>
+        <v>12802</v>
       </c>
       <c r="J56" t="inlineStr"/>
     </row>
@@ -2220,24 +2164,24 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
-        <v>31556</v>
+        <v>31945</v>
       </c>
       <c r="H57" t="n">
-        <v>17718</v>
+        <v>19159</v>
       </c>
       <c r="I57" t="n">
-        <v>15961</v>
+        <v>14138</v>
       </c>
       <c r="J57" t="inlineStr"/>
     </row>
@@ -2250,24 +2194,24 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
-        <v>33155</v>
+        <v>30362</v>
       </c>
       <c r="H58" t="n">
-        <v>12151</v>
+        <v>15887</v>
       </c>
       <c r="I58" t="n">
-        <v>16283</v>
+        <v>17908</v>
       </c>
       <c r="J58" t="inlineStr"/>
     </row>
@@ -2280,24 +2224,24 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
-        <v>34855</v>
+        <v>34234</v>
       </c>
       <c r="H59" t="n">
-        <v>15245</v>
+        <v>14195</v>
       </c>
       <c r="I59" t="n">
-        <v>15681</v>
+        <v>14686</v>
       </c>
       <c r="J59" t="inlineStr"/>
     </row>
@@ -2310,24 +2254,24 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
-        <v>31150</v>
+        <v>33096</v>
       </c>
       <c r="H60" t="n">
-        <v>16896</v>
+        <v>15993</v>
       </c>
       <c r="I60" t="n">
-        <v>10242</v>
+        <v>18664</v>
       </c>
       <c r="J60" t="inlineStr"/>
     </row>
@@ -2340,24 +2284,24 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
-        <v>34948</v>
+        <v>34886</v>
       </c>
       <c r="H61" t="n">
-        <v>13458</v>
+        <v>16377</v>
       </c>
       <c r="I61" t="n">
-        <v>15293</v>
+        <v>16552</v>
       </c>
       <c r="J61" t="inlineStr"/>
     </row>
@@ -2370,24 +2314,24 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
-        <v>30203</v>
+        <v>28624</v>
       </c>
       <c r="H62" t="n">
-        <v>19833</v>
+        <v>10114</v>
       </c>
       <c r="I62" t="n">
-        <v>19560</v>
+        <v>14594</v>
       </c>
       <c r="J62" t="inlineStr"/>
     </row>
@@ -2400,24 +2344,24 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
-        <v>34130</v>
+        <v>28799</v>
       </c>
       <c r="H63" t="n">
-        <v>13734</v>
+        <v>13708</v>
       </c>
       <c r="I63" t="n">
-        <v>15334</v>
+        <v>17749</v>
       </c>
       <c r="J63" t="inlineStr"/>
     </row>
@@ -2430,24 +2374,24 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="n">
-        <v>25033</v>
+        <v>29075</v>
       </c>
       <c r="H64" t="n">
-        <v>19326</v>
+        <v>16227</v>
       </c>
       <c r="I64" t="n">
-        <v>14913</v>
+        <v>16141</v>
       </c>
       <c r="J64" t="inlineStr"/>
     </row>
@@ -2460,24 +2404,24 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="n">
-        <v>26119</v>
+        <v>30253</v>
       </c>
       <c r="H65" t="n">
-        <v>10892</v>
+        <v>13602</v>
       </c>
       <c r="I65" t="n">
-        <v>12618</v>
+        <v>12007</v>
       </c>
       <c r="J65" t="inlineStr"/>
     </row>
@@ -2490,24 +2434,24 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
-        <v>28273</v>
+        <v>34693</v>
       </c>
       <c r="H66" t="n">
-        <v>11758</v>
+        <v>19747</v>
       </c>
       <c r="I66" t="n">
-        <v>18554</v>
+        <v>18143</v>
       </c>
       <c r="J66" t="inlineStr"/>
     </row>
@@ -2520,24 +2464,24 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
-        <v>26724</v>
+        <v>31421</v>
       </c>
       <c r="H67" t="n">
-        <v>18982</v>
+        <v>13174</v>
       </c>
       <c r="I67" t="n">
-        <v>19428</v>
+        <v>11854</v>
       </c>
       <c r="J67" t="inlineStr"/>
     </row>
@@ -2550,24 +2494,24 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="n">
-        <v>33240</v>
+        <v>30393</v>
       </c>
       <c r="H68" t="n">
-        <v>10281</v>
+        <v>10960</v>
       </c>
       <c r="I68" t="n">
-        <v>17391</v>
+        <v>19598</v>
       </c>
       <c r="J68" t="inlineStr"/>
     </row>
@@ -2580,24 +2524,24 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="n">
-        <v>34148</v>
+        <v>31977</v>
       </c>
       <c r="H69" t="n">
-        <v>16217</v>
+        <v>10173</v>
       </c>
       <c r="I69" t="n">
-        <v>10610</v>
+        <v>19797</v>
       </c>
       <c r="J69" t="inlineStr"/>
     </row>
@@ -2610,24 +2554,24 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="n">
-        <v>32762</v>
+        <v>27912</v>
       </c>
       <c r="H70" t="n">
-        <v>16079</v>
+        <v>17247</v>
       </c>
       <c r="I70" t="n">
-        <v>13585</v>
+        <v>11248</v>
       </c>
       <c r="J70" t="inlineStr"/>
     </row>
@@ -2640,24 +2584,24 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="n">
-        <v>34074</v>
+        <v>31783</v>
       </c>
       <c r="H71" t="n">
-        <v>15164</v>
+        <v>18719</v>
       </c>
       <c r="I71" t="n">
-        <v>10164</v>
+        <v>13673</v>
       </c>
       <c r="J71" t="inlineStr"/>
     </row>
@@ -2681,13 +2625,13 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="n">
-        <v>32671</v>
+        <v>26286</v>
       </c>
       <c r="H72" t="n">
-        <v>14355</v>
+        <v>14377</v>
       </c>
       <c r="I72" t="n">
-        <v>10029</v>
+        <v>18775</v>
       </c>
       <c r="J72" t="inlineStr"/>
     </row>
@@ -2700,24 +2644,24 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="n">
-        <v>32777</v>
+        <v>26723</v>
       </c>
       <c r="H73" t="n">
-        <v>10387</v>
+        <v>15497</v>
       </c>
       <c r="I73" t="n">
-        <v>12987</v>
+        <v>14973</v>
       </c>
       <c r="J73" t="inlineStr"/>
     </row>
@@ -2730,24 +2674,24 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="n">
-        <v>31866</v>
+        <v>34148</v>
       </c>
       <c r="H74" t="n">
-        <v>18978</v>
+        <v>18896</v>
       </c>
       <c r="I74" t="n">
-        <v>17861</v>
+        <v>16536</v>
       </c>
       <c r="J74" t="inlineStr"/>
     </row>
@@ -2760,24 +2704,24 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="n">
-        <v>26019</v>
+        <v>31370</v>
       </c>
       <c r="H75" t="n">
-        <v>16918</v>
+        <v>14781</v>
       </c>
       <c r="I75" t="n">
-        <v>15347</v>
+        <v>18816</v>
       </c>
       <c r="J75" t="inlineStr"/>
     </row>
@@ -2790,24 +2734,24 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="n">
-        <v>28252</v>
+        <v>33280</v>
       </c>
       <c r="H76" t="n">
-        <v>14924</v>
+        <v>10569</v>
       </c>
       <c r="I76" t="n">
-        <v>16117</v>
+        <v>10822</v>
       </c>
       <c r="J76" t="inlineStr"/>
     </row>
@@ -2820,24 +2764,24 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="n">
-        <v>26349</v>
+        <v>34435</v>
       </c>
       <c r="H77" t="n">
-        <v>15973</v>
+        <v>12071</v>
       </c>
       <c r="I77" t="n">
-        <v>18514</v>
+        <v>13409</v>
       </c>
       <c r="J77" t="inlineStr"/>
     </row>
@@ -2850,24 +2794,24 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>water</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>fruit</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="n">
-        <v>30870</v>
+        <v>27725</v>
       </c>
       <c r="H78" t="n">
-        <v>18688</v>
+        <v>14283</v>
       </c>
       <c r="I78" t="n">
-        <v>18017</v>
+        <v>18983</v>
       </c>
       <c r="J78" t="inlineStr"/>
     </row>
@@ -2880,24 +2824,24 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>fruit</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="n">
-        <v>29594</v>
+        <v>25063</v>
       </c>
       <c r="H79" t="n">
-        <v>17199</v>
+        <v>12520</v>
       </c>
       <c r="I79" t="n">
-        <v>17036</v>
+        <v>15925</v>
       </c>
       <c r="J79" t="inlineStr"/>
     </row>
@@ -2921,13 +2865,13 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="n">
-        <v>29454</v>
+        <v>28351</v>
       </c>
       <c r="H80" t="n">
-        <v>11021</v>
+        <v>12571</v>
       </c>
       <c r="I80" t="n">
-        <v>12570</v>
+        <v>14472</v>
       </c>
       <c r="J80" t="inlineStr"/>
     </row>
@@ -2940,24 +2884,24 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>lemon</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>cake</t>
+          <t>lime</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="n">
-        <v>26212</v>
+        <v>26857</v>
       </c>
       <c r="H81" t="n">
-        <v>13500</v>
+        <v>16151</v>
       </c>
       <c r="I81" t="n">
-        <v>15225</v>
+        <v>11782</v>
       </c>
       <c r="J81" t="inlineStr"/>
     </row>

</xml_diff>